<commit_message>
Removed CNP from Raiffeisen MTA
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/templates/MTA_Raiffeisen.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/templates/MTA_Raiffeisen.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandru POP\Desktop\Proiecte\webapp-spring\server\src\main\java\net\guides\springboot2\crud\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="9948"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Descriere tranzactie cont platitor</t>
   </si>
@@ -29,9 +34,6 @@
   </si>
   <si>
     <t>Suma</t>
-  </si>
-  <si>
-    <t>CNP/CUI beneficiar</t>
   </si>
   <si>
     <t>Nume beneficiar</t>
@@ -430,7 +432,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -441,10 +443,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -452,39 +454,38 @@
     <col min="1" max="1" width="39.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.85546875" style="5" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="17" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" style="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="5"/>
+    <col min="4" max="4" width="18.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="15" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" style="15" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
       <c r="J1" s="5"/>
@@ -498,9 +499,8 @@
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -508,8 +508,8 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -523,9 +523,8 @@
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -535,16 +534,14 @@
       <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
@@ -558,16 +555,15 @@
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -581,16 +577,15 @@
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
@@ -604,16 +599,15 @@
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -627,16 +621,15 @@
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
-      <c r="U6" s="5"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -650,16 +643,15 @@
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
-      <c r="U7" s="5"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -673,16 +665,15 @@
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
+      <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -696,16 +687,15 @@
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
       <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
+      <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -719,16 +709,15 @@
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
       <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -742,16 +731,15 @@
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
       <c r="T11" s="5"/>
-      <c r="U11" s="5"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
@@ -765,16 +753,15 @@
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
       <c r="T12" s="5"/>
-      <c r="U12" s="5"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
@@ -788,16 +775,15 @@
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
       <c r="T13" s="5"/>
-      <c r="U13" s="5"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
+      <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -811,16 +797,15 @@
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
       <c r="T14" s="5"/>
-      <c r="U14" s="5"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -834,16 +819,15 @@
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
       <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -857,16 +841,15 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -880,16 +863,15 @@
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="5"/>
-      <c r="U17" s="5"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="G18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
@@ -903,16 +885,15 @@
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="5"/>
-      <c r="U18" s="5"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -926,16 +907,15 @@
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
       <c r="T19" s="5"/>
-      <c r="U19" s="5"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="G20" s="5"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
@@ -949,14 +929,13 @@
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
       <c r="T20" s="5"/>
-      <c r="U20" s="5"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="9"/>
       <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
@@ -972,14 +951,13 @@
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
       <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="12"/>
       <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
+      <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -995,15 +973,14 @@
       <c r="R22" s="14"/>
       <c r="S22" s="14"/>
       <c r="T22" s="14"/>
-      <c r="U22" s="14"/>
-      <c r="V22" s="11"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="U22" s="11"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="11"/>
       <c r="C23" s="12"/>
       <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
+      <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
@@ -1019,15 +996,14 @@
       <c r="R23" s="14"/>
       <c r="S23" s="14"/>
       <c r="T23" s="14"/>
-      <c r="U23" s="14"/>
-      <c r="V23" s="11"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="U23" s="11"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="B24" s="11"/>
       <c r="C24" s="12"/>
       <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
+      <c r="E24" s="14"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
@@ -1043,15 +1019,14 @@
       <c r="R24" s="14"/>
       <c r="S24" s="14"/>
       <c r="T24" s="14"/>
-      <c r="U24" s="14"/>
-      <c r="V24" s="11"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="U24" s="11"/>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="11"/>
       <c r="C25" s="12"/>
       <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
+      <c r="E25" s="14"/>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
@@ -1067,15 +1042,14 @@
       <c r="R25" s="14"/>
       <c r="S25" s="14"/>
       <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
-      <c r="V25" s="11"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="U25" s="11"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="11"/>
       <c r="C26" s="12"/>
       <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
+      <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
@@ -1091,14 +1065,13 @@
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
       <c r="T26" s="14"/>
-      <c r="U26" s="14"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="11"/>
       <c r="C27" s="12"/>
       <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
+      <c r="E27" s="14"/>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
@@ -1114,14 +1087,13 @@
       <c r="R27" s="14"/>
       <c r="S27" s="14"/>
       <c r="T27" s="14"/>
-      <c r="U27" s="14"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="11"/>
       <c r="C28" s="12"/>
       <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
+      <c r="E28" s="14"/>
       <c r="F28" s="14"/>
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
@@ -1137,14 +1109,13 @@
       <c r="R28" s="14"/>
       <c r="S28" s="14"/>
       <c r="T28" s="14"/>
-      <c r="U28" s="14"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="11"/>
       <c r="C29" s="12"/>
       <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
+      <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
@@ -1160,14 +1131,13 @@
       <c r="R29" s="14"/>
       <c r="S29" s="14"/>
       <c r="T29" s="14"/>
-      <c r="U29" s="14"/>
-    </row>
-    <row r="30" spans="1:22" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:21" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="B30" s="11"/>
       <c r="C30" s="12"/>
       <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
+      <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
@@ -1183,14 +1153,13 @@
       <c r="R30" s="14"/>
       <c r="S30" s="14"/>
       <c r="T30" s="14"/>
-      <c r="U30" s="14"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="11"/>
       <c r="C31" s="12"/>
       <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
+      <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
@@ -1205,7 +1174,6 @@
       <c r="Q31" s="14"/>
       <c r="R31" s="14"/>
       <c r="S31" s="14"/>
-      <c r="T31" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>